<commit_message>
dados natureza e tipo
</commit_message>
<xml_diff>
--- a/SUR SUR-lag SUR-error/tidy_agredados_ssp.xlsx
+++ b/SUR SUR-lag SUR-error/tidy_agredados_ssp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20055" windowHeight="9225"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="20055" windowHeight="9225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -282,12 +282,6 @@
     <t>Outros delitos (Inclui contravenções)</t>
   </si>
   <si>
-    <t>Outros criminais (não inclui contravenções)</t>
-  </si>
-  <si>
-    <t>Contravencionais</t>
-  </si>
-  <si>
     <t>Entorpecentes</t>
   </si>
   <si>
@@ -298,9 +292,6 @@
   </si>
   <si>
     <t>Contra a pessoa</t>
-  </si>
-  <si>
-    <t>Ocorrências policiais registradas, por natureza</t>
   </si>
   <si>
     <t>Ocorrência/período</t>
@@ -363,16 +354,25 @@
     <t>grupo</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>2005-2T</t>
   </si>
   <si>
-    <t>Roubo NA outros (6) (i)</t>
+    <t>Contravencio-is</t>
   </si>
   <si>
-    <t>Furto NA outros</t>
+    <t>Outros crimi-is (não inclui contravenções)</t>
   </si>
   <si>
-    <t>2005-2T</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Ocorrências policiais registradas, por -tureza</t>
+  </si>
+  <si>
+    <t>Roubo - outros (6) (i)</t>
+  </si>
+  <si>
+    <t>Furto - outros</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E235" sqref="E235"/>
     </sheetView>
   </sheetViews>
@@ -754,28 +754,28 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>87</v>
@@ -787,7 +787,7 @@
         <v>85</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -825,7 +825,7 @@
         <v>100118</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -863,7 +863,7 @@
         <v>51087</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -901,7 +901,7 @@
         <v>170907</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -939,7 +939,7 @@
         <v>91066</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -977,7 +977,7 @@
         <v>45028</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1015,7 +1015,7 @@
         <v>168462</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1053,7 +1053,7 @@
         <v>78241</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1091,7 +1091,7 @@
         <v>43248</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1129,7 +1129,7 @@
         <v>172268</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1167,7 +1167,7 @@
         <v>85342</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1205,7 +1205,7 @@
         <v>45842</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1243,7 +1243,7 @@
         <v>173312</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1281,7 +1281,7 @@
         <v>87811</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1319,7 +1319,7 @@
         <v>45151</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1357,7 +1357,7 @@
         <v>175510</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1395,7 +1395,7 @@
         <v>86127</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1433,7 +1433,7 @@
         <v>44774</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1471,7 +1471,7 @@
         <v>185986</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1509,7 +1509,7 @@
         <v>90740</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1547,7 +1547,7 @@
         <v>49954</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1585,7 +1585,7 @@
         <v>189105</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1623,7 +1623,7 @@
         <v>99354</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1661,7 +1661,7 @@
         <v>52436</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1699,7 +1699,7 @@
         <v>192663</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1737,7 +1737,7 @@
         <v>104354</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1775,7 +1775,7 @@
         <v>54022</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1813,7 +1813,7 @@
         <v>205556</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1851,7 +1851,7 @@
         <v>108936</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1889,7 +1889,7 @@
         <v>57408</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1927,7 +1927,7 @@
         <v>213083</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1965,7 +1965,7 @@
         <v>111857</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2003,7 +2003,7 @@
         <v>57660</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2041,7 +2041,7 @@
         <v>218531</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2079,7 +2079,7 @@
         <v>113519</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2117,7 +2117,7 @@
         <v>58194</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2155,7 +2155,7 @@
         <v>207285</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2193,7 +2193,7 @@
         <v>120483</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2231,7 +2231,7 @@
         <v>61663</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2269,7 +2269,7 @@
         <v>213040</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2307,7 +2307,7 @@
         <v>128680</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2345,7 +2345,7 @@
         <v>67746</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2383,7 +2383,7 @@
         <v>229576</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2421,7 +2421,7 @@
         <v>128570</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2459,7 +2459,7 @@
         <v>71685</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2497,7 +2497,7 @@
         <v>236583</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2535,7 +2535,7 @@
         <v>134580</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -2573,7 +2573,7 @@
         <v>76244</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2611,7 +2611,7 @@
         <v>232654</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2649,7 +2649,7 @@
         <v>131943</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2687,7 +2687,7 @@
         <v>72008</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -2725,7 +2725,7 @@
         <v>231203</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -2763,7 +2763,7 @@
         <v>128303</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -2801,7 +2801,7 @@
         <v>71231</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -2839,7 +2839,7 @@
         <v>234800</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -2877,7 +2877,7 @@
         <v>127101</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -2915,7 +2915,7 @@
         <v>66205</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -2953,7 +2953,7 @@
         <v>242479</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -2991,7 +2991,7 @@
         <v>128721</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -3029,7 +3029,7 @@
         <v>71202</v>
       </c>
       <c r="L60" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3067,7 +3067,7 @@
         <v>237578</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3105,7 +3105,7 @@
         <v>128558</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -3143,7 +3143,7 @@
         <v>69444</v>
       </c>
       <c r="L63" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3181,7 +3181,7 @@
         <v>232445</v>
       </c>
       <c r="L64" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -3219,7 +3219,7 @@
         <v>128642</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -3257,7 +3257,7 @@
         <v>71251</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3295,7 +3295,7 @@
         <v>241803</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -3333,7 +3333,7 @@
         <v>125620</v>
       </c>
       <c r="L68" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -3371,7 +3371,7 @@
         <v>69950</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -3409,7 +3409,7 @@
         <v>242862</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -3447,7 +3447,7 @@
         <v>125945</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -3485,7 +3485,7 @@
         <v>70126</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -3523,7 +3523,7 @@
         <v>240824</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -3561,7 +3561,7 @@
         <v>125461</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -3599,7 +3599,7 @@
         <v>69661</v>
       </c>
       <c r="L75" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -3637,7 +3637,7 @@
         <v>234600</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -3675,7 +3675,7 @@
         <v>127744</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -3713,7 +3713,7 @@
         <v>72034</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -3751,7 +3751,7 @@
         <v>244251</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -3789,7 +3789,7 @@
         <v>126641</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -3827,7 +3827,7 @@
         <v>68742</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -3865,7 +3865,7 @@
         <v>237683</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -3903,7 +3903,7 @@
         <v>130793</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -3941,7 +3941,7 @@
         <v>71434</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -3979,7 +3979,7 @@
         <v>240487</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -4017,7 +4017,7 @@
         <v>126064</v>
       </c>
       <c r="L86" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -4055,7 +4055,7 @@
         <v>68537</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -4093,7 +4093,7 @@
         <v>234110</v>
       </c>
       <c r="L88" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -4131,7 +4131,7 @@
         <v>138009</v>
       </c>
       <c r="L89" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -4169,7 +4169,7 @@
         <v>74599</v>
       </c>
       <c r="L90" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -4207,7 +4207,7 @@
         <v>262338</v>
       </c>
       <c r="L91" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -4245,7 +4245,7 @@
         <v>140058</v>
       </c>
       <c r="L92" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -4283,7 +4283,7 @@
         <v>74582</v>
       </c>
       <c r="L93" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -4321,7 +4321,7 @@
         <v>265448</v>
       </c>
       <c r="L94" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -4359,7 +4359,7 @@
         <v>143698</v>
       </c>
       <c r="L95" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -4397,7 +4397,7 @@
         <v>75960</v>
       </c>
       <c r="L96" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -4435,7 +4435,7 @@
         <v>265217</v>
       </c>
       <c r="L97" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -4473,7 +4473,7 @@
         <v>146862</v>
       </c>
       <c r="L98" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -4511,7 +4511,7 @@
         <v>75092</v>
       </c>
       <c r="L99" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -4549,7 +4549,7 @@
         <v>266046</v>
       </c>
       <c r="L100" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -4587,7 +4587,7 @@
         <v>146386</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -4625,7 +4625,7 @@
         <v>74808</v>
       </c>
       <c r="L102" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -4663,7 +4663,7 @@
         <v>271184</v>
       </c>
       <c r="L103" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:12">
@@ -4701,7 +4701,7 @@
         <v>142359</v>
       </c>
       <c r="L104" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -4739,7 +4739,7 @@
         <v>72018</v>
       </c>
       <c r="L105" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:12">
@@ -4777,7 +4777,7 @@
         <v>267764</v>
       </c>
       <c r="L106" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:12">
@@ -4815,7 +4815,7 @@
         <v>147890</v>
       </c>
       <c r="L107" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:12">
@@ -4853,7 +4853,7 @@
         <v>73289</v>
       </c>
       <c r="L108" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:12">
@@ -4891,7 +4891,7 @@
         <v>264601</v>
       </c>
       <c r="L109" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:12">
@@ -4930,7 +4930,7 @@
         <v>148190</v>
       </c>
       <c r="L110" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="111" spans="1:12">
@@ -4968,7 +4968,7 @@
         <v>76098</v>
       </c>
       <c r="L111" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:12">
@@ -5006,7 +5006,7 @@
         <v>274436</v>
       </c>
       <c r="L112" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:12">
@@ -5044,7 +5044,7 @@
         <v>145655</v>
       </c>
       <c r="L113" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:12">
@@ -5082,7 +5082,7 @@
         <v>76335</v>
       </c>
       <c r="L114" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:12">
@@ -5120,7 +5120,7 @@
         <v>281164</v>
       </c>
       <c r="L115" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -5158,7 +5158,7 @@
         <v>140420</v>
       </c>
       <c r="L116" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -5196,7 +5196,7 @@
         <v>74966</v>
       </c>
       <c r="L117" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:12">
@@ -5234,12 +5234,12 @@
         <v>283509</v>
       </c>
       <c r="L118" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>3</v>
@@ -5272,12 +5272,12 @@
         <v>149949</v>
       </c>
       <c r="L119" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="120" spans="1:12">
       <c r="A120" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>2</v>
@@ -5310,12 +5310,12 @@
         <v>78188</v>
       </c>
       <c r="L120" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:12">
       <c r="A121" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>0</v>
@@ -5348,7 +5348,7 @@
         <v>280088</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="1:12">
@@ -5386,7 +5386,7 @@
         <v>148916</v>
       </c>
       <c r="L122" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:12">
@@ -5424,7 +5424,7 @@
         <v>77378</v>
       </c>
       <c r="L123" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="1:12">
@@ -5462,7 +5462,7 @@
         <v>280107</v>
       </c>
       <c r="L124" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="125" spans="1:12">
@@ -5500,7 +5500,7 @@
         <v>142704</v>
       </c>
       <c r="L125" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="1:12">
@@ -5538,7 +5538,7 @@
         <v>73995</v>
       </c>
       <c r="L126" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="127" spans="1:12">
@@ -5576,7 +5576,7 @@
         <v>279367</v>
       </c>
       <c r="L127" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="128" spans="1:12">
@@ -5614,7 +5614,7 @@
         <v>143886</v>
       </c>
       <c r="L128" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:12">
@@ -5652,7 +5652,7 @@
         <v>74836</v>
       </c>
       <c r="L129" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="130" spans="1:12">
@@ -5690,7 +5690,7 @@
         <v>283701</v>
       </c>
       <c r="L130" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -5728,7 +5728,7 @@
         <v>147964</v>
       </c>
       <c r="L131" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="132" spans="1:12">
@@ -5766,7 +5766,7 @@
         <v>72519</v>
       </c>
       <c r="L132" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="133" spans="1:12">
@@ -5804,7 +5804,7 @@
         <v>268941</v>
       </c>
       <c r="L133" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="134" spans="1:12">
@@ -5842,7 +5842,7 @@
         <v>146133</v>
       </c>
       <c r="L134" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="135" spans="1:12">
@@ -5880,7 +5880,7 @@
         <v>74187</v>
       </c>
       <c r="L135" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="136" spans="1:12">
@@ -5918,7 +5918,7 @@
         <v>270340</v>
       </c>
       <c r="L136" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="137" spans="1:12">
@@ -5956,7 +5956,7 @@
         <v>141055</v>
       </c>
       <c r="L137" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="138" spans="1:12">
@@ -5994,7 +5994,7 @@
         <v>74405</v>
       </c>
       <c r="L138" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -6032,7 +6032,7 @@
         <v>280851</v>
       </c>
       <c r="L139" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="140" spans="1:12">
@@ -6070,7 +6070,7 @@
         <v>142502</v>
       </c>
       <c r="L140" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="141" spans="1:12">
@@ -6108,7 +6108,7 @@
         <v>76099</v>
       </c>
       <c r="L141" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="142" spans="1:12">
@@ -6146,7 +6146,7 @@
         <v>284876</v>
       </c>
       <c r="L142" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="143" spans="1:12">
@@ -6184,7 +6184,7 @@
         <v>147488</v>
       </c>
       <c r="L143" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="144" spans="1:12">
@@ -6222,7 +6222,7 @@
         <v>76019</v>
       </c>
       <c r="L144" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" spans="1:12">
@@ -6260,7 +6260,7 @@
         <v>278157</v>
       </c>
       <c r="L145" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="146" spans="1:12">
@@ -6298,7 +6298,7 @@
         <v>139479</v>
       </c>
       <c r="L146" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="147" spans="1:12">
@@ -6336,7 +6336,7 @@
         <v>77656</v>
       </c>
       <c r="L147" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="148" spans="1:12">
@@ -6374,7 +6374,7 @@
         <v>278882</v>
       </c>
       <c r="L148" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="149" spans="1:12">
@@ -6412,7 +6412,7 @@
         <v>134079</v>
       </c>
       <c r="L149" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="150" spans="1:12">
@@ -6450,7 +6450,7 @@
         <v>78520</v>
       </c>
       <c r="L150" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="151" spans="1:12">
@@ -6488,7 +6488,7 @@
         <v>280391</v>
       </c>
       <c r="L151" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="152" spans="1:12">
@@ -6526,7 +6526,7 @@
         <v>137399</v>
       </c>
       <c r="L152" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="153" spans="1:12">
@@ -6564,7 +6564,7 @@
         <v>79883</v>
       </c>
       <c r="L153" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="154" spans="1:12">
@@ -6602,7 +6602,7 @@
         <v>277382</v>
       </c>
       <c r="L154" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="155" spans="1:12">
@@ -6640,7 +6640,7 @@
         <v>149406</v>
       </c>
       <c r="L155" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="156" spans="1:12">
@@ -6678,7 +6678,7 @@
         <v>80514</v>
       </c>
       <c r="L156" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="157" spans="1:12">
@@ -6716,7 +6716,7 @@
         <v>270096</v>
       </c>
       <c r="L157" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="158" spans="1:12">
@@ -6754,7 +6754,7 @@
         <v>146793</v>
       </c>
       <c r="L158" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="159" spans="1:12">
@@ -6792,7 +6792,7 @@
         <v>77162</v>
       </c>
       <c r="L159" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="160" spans="1:12">
@@ -6830,7 +6830,7 @@
         <v>238970</v>
       </c>
       <c r="L160" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="161" spans="1:12">
@@ -6868,7 +6868,7 @@
         <v>123108</v>
       </c>
       <c r="L161" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="162" spans="1:12">
@@ -6906,7 +6906,7 @@
         <v>68844</v>
       </c>
       <c r="L162" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="163" spans="1:12">
@@ -6944,7 +6944,7 @@
         <v>203746</v>
       </c>
       <c r="L163" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="164" spans="1:12">
@@ -6982,7 +6982,7 @@
         <v>146945</v>
       </c>
       <c r="L164" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="165" spans="1:12">
@@ -7020,7 +7020,7 @@
         <v>81239</v>
       </c>
       <c r="L165" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="166" spans="1:12">
@@ -7058,7 +7058,7 @@
         <v>277996</v>
       </c>
       <c r="L166" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="167" spans="1:12">
@@ -7096,7 +7096,7 @@
         <v>153204</v>
       </c>
       <c r="L167" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="168" spans="1:12">
@@ -7134,7 +7134,7 @@
         <v>83429</v>
       </c>
       <c r="L168" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="169" spans="1:12">
@@ -7172,7 +7172,7 @@
         <v>275863</v>
       </c>
       <c r="L169" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="170" spans="1:12">
@@ -7210,7 +7210,7 @@
         <v>150026</v>
       </c>
       <c r="L170" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="171" spans="1:12">
@@ -7248,7 +7248,7 @@
         <v>80512</v>
       </c>
       <c r="L171" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="172" spans="1:12">
@@ -7286,7 +7286,7 @@
         <v>268809</v>
       </c>
       <c r="L172" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="173" spans="1:12">
@@ -7324,7 +7324,7 @@
         <v>148250</v>
       </c>
       <c r="L173" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="174" spans="1:12">
@@ -7362,7 +7362,7 @@
         <v>80385</v>
       </c>
       <c r="L174" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="175" spans="1:12">
@@ -7400,7 +7400,7 @@
         <v>278023</v>
       </c>
       <c r="L175" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="176" spans="1:12">
@@ -7438,7 +7438,7 @@
         <v>136714</v>
       </c>
       <c r="L176" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="177" spans="1:12">
@@ -7476,7 +7476,7 @@
         <v>76805</v>
       </c>
       <c r="L177" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="178" spans="1:12">
@@ -7514,7 +7514,7 @@
         <v>269971</v>
       </c>
       <c r="L178" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="179" spans="1:12">
@@ -7552,7 +7552,7 @@
         <v>140840</v>
       </c>
       <c r="L179" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="180" spans="1:12">
@@ -7590,7 +7590,7 @@
         <v>76406</v>
       </c>
       <c r="L180" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="181" spans="1:12">
@@ -7628,7 +7628,7 @@
         <v>260368</v>
       </c>
       <c r="L181" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="182" spans="1:12">
@@ -7666,7 +7666,7 @@
         <v>150550</v>
       </c>
       <c r="L182" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="183" spans="1:12">
@@ -7704,7 +7704,7 @@
         <v>79309</v>
       </c>
       <c r="L183" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="184" spans="1:12">
@@ -7742,7 +7742,7 @@
         <v>265568</v>
       </c>
       <c r="L184" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="185" spans="1:12">
@@ -7780,7 +7780,7 @@
         <v>145042</v>
       </c>
       <c r="L185" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="186" spans="1:12">
@@ -7818,7 +7818,7 @@
         <v>78199</v>
       </c>
       <c r="L186" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="187" spans="1:12">
@@ -7856,7 +7856,7 @@
         <v>269041</v>
       </c>
       <c r="L187" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="188" spans="1:12">
@@ -7894,7 +7894,7 @@
         <v>148580</v>
       </c>
       <c r="L188" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="189" spans="1:12">
@@ -7932,7 +7932,7 @@
         <v>81118</v>
       </c>
       <c r="L189" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="190" spans="1:12">
@@ -7970,7 +7970,7 @@
         <v>273758</v>
       </c>
       <c r="L190" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="191" spans="1:12">
@@ -8008,7 +8008,7 @@
         <v>157895</v>
       </c>
       <c r="L191" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="192" spans="1:12">
@@ -8046,7 +8046,7 @@
         <v>83389</v>
       </c>
       <c r="L192" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="193" spans="1:12">
@@ -8084,7 +8084,7 @@
         <v>275594</v>
       </c>
       <c r="L193" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="194" spans="1:12">
@@ -8122,7 +8122,7 @@
         <v>161758</v>
       </c>
       <c r="L194" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="195" spans="1:12">
@@ -8160,7 +8160,7 @@
         <v>84635</v>
       </c>
       <c r="L195" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="196" spans="1:12">
@@ -8198,7 +8198,7 @@
         <v>280552</v>
       </c>
       <c r="L196" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="197" spans="1:12">
@@ -8236,7 +8236,7 @@
         <v>159720</v>
       </c>
       <c r="L197" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="198" spans="1:12">
@@ -8274,7 +8274,7 @@
         <v>83621</v>
       </c>
       <c r="L198" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="199" spans="1:12">
@@ -8312,7 +8312,7 @@
         <v>275713</v>
       </c>
       <c r="L199" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="200" spans="1:12">
@@ -8350,7 +8350,7 @@
         <v>162033</v>
       </c>
       <c r="L200" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="201" spans="1:12">
@@ -8388,7 +8388,7 @@
         <v>85629</v>
       </c>
       <c r="L201" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="202" spans="1:12">
@@ -8426,7 +8426,7 @@
         <v>288628</v>
       </c>
       <c r="L202" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="203" spans="1:12">
@@ -8464,7 +8464,7 @@
         <v>168868</v>
       </c>
       <c r="L203" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="204" spans="1:12">
@@ -8502,7 +8502,7 @@
         <v>87752</v>
       </c>
       <c r="L204" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="205" spans="1:12">
@@ -8540,7 +8540,7 @@
         <v>278072</v>
       </c>
       <c r="L205" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="206" spans="1:12">
@@ -8578,7 +8578,7 @@
         <v>166039</v>
       </c>
       <c r="L206" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="207" spans="1:12">
@@ -8616,7 +8616,7 @@
         <v>88799</v>
       </c>
       <c r="L207" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="208" spans="1:12">
@@ -8654,7 +8654,7 @@
         <v>286308</v>
       </c>
       <c r="L208" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="209" spans="1:12">
@@ -8692,7 +8692,7 @@
         <v>164821</v>
       </c>
       <c r="L209" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="210" spans="1:12">
@@ -8730,7 +8730,7 @@
         <v>87218</v>
       </c>
       <c r="L210" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="211" spans="1:12">
@@ -8768,7 +8768,7 @@
         <v>288550</v>
       </c>
       <c r="L211" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="212" spans="1:12">
@@ -8806,7 +8806,7 @@
         <v>163799</v>
       </c>
       <c r="L212" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="213" spans="1:12">
@@ -8844,7 +8844,7 @@
         <v>87477</v>
       </c>
       <c r="L213" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="214" spans="1:12">
@@ -8882,7 +8882,7 @@
         <v>286528</v>
       </c>
       <c r="L214" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="215" spans="1:12">
@@ -8920,7 +8920,7 @@
         <v>171733</v>
       </c>
       <c r="L215" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="216" spans="1:12">
@@ -8958,7 +8958,7 @@
         <v>90070</v>
       </c>
       <c r="L216" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="217" spans="1:12">
@@ -8996,7 +8996,7 @@
         <v>283569</v>
       </c>
       <c r="L217" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="218" spans="1:12">
@@ -9034,7 +9034,7 @@
         <v>167313</v>
       </c>
       <c r="L218" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="219" spans="1:12">
@@ -9072,7 +9072,7 @@
         <v>88086</v>
       </c>
       <c r="L219" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="220" spans="1:12">
@@ -9110,7 +9110,7 @@
         <v>271949</v>
       </c>
       <c r="L220" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="221" spans="1:12">
@@ -9148,7 +9148,7 @@
         <v>164650</v>
       </c>
       <c r="L221" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="222" spans="1:12">
@@ -9186,7 +9186,7 @@
         <v>85114</v>
       </c>
       <c r="L222" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="223" spans="1:12">
@@ -9224,7 +9224,7 @@
         <v>268677</v>
       </c>
       <c r="L223" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="224" spans="1:12">
@@ -9262,7 +9262,7 @@
         <v>168062</v>
       </c>
       <c r="L224" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="225" spans="1:12">
@@ -9300,7 +9300,7 @@
         <v>88679</v>
       </c>
       <c r="L225" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="226" spans="1:12">
@@ -9338,7 +9338,7 @@
         <v>280071</v>
       </c>
       <c r="L226" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="227" spans="1:12">
@@ -9376,7 +9376,7 @@
         <v>170315</v>
       </c>
       <c r="L227" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="228" spans="1:12">
@@ -9414,7 +9414,7 @@
         <v>86311</v>
       </c>
       <c r="L228" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="229" spans="1:12">
@@ -9452,7 +9452,7 @@
         <v>263749</v>
       </c>
       <c r="L229" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="230" spans="1:12">
@@ -9490,7 +9490,7 @@
         <v>161248</v>
       </c>
       <c r="L230" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="231" spans="1:12">
@@ -9528,7 +9528,7 @@
         <v>82863</v>
       </c>
       <c r="L231" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="232" spans="1:12">
@@ -9566,7 +9566,7 @@
         <v>259243</v>
       </c>
       <c r="L232" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="233" spans="1:12">
@@ -9604,7 +9604,7 @@
         <v>156877</v>
       </c>
       <c r="L233" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="234" spans="1:12">
@@ -9642,7 +9642,7 @@
         <v>81160</v>
       </c>
       <c r="L234" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="235" spans="1:12">
@@ -9680,7 +9680,7 @@
         <v>257750</v>
       </c>
       <c r="L235" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="236" spans="1:12">
@@ -9718,7 +9718,7 @@
         <v>151613</v>
       </c>
       <c r="L236" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="237" spans="1:12">
@@ -9756,7 +9756,7 @@
         <v>80847</v>
       </c>
       <c r="L237" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="238" spans="1:12">
@@ -9794,7 +9794,7 @@
         <v>250858</v>
       </c>
       <c r="L238" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="239" spans="1:12">
@@ -9832,7 +9832,7 @@
         <v>148241</v>
       </c>
       <c r="L239" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="240" spans="1:12">
@@ -9870,7 +9870,7 @@
         <v>77919</v>
       </c>
       <c r="L240" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="241" spans="1:12">
@@ -9908,7 +9908,7 @@
         <v>250118</v>
       </c>
       <c r="L241" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="242" spans="1:12">
@@ -9946,7 +9946,7 @@
         <v>150782</v>
       </c>
       <c r="L242" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="243" spans="1:12">
@@ -9984,7 +9984,7 @@
         <v>81493</v>
       </c>
       <c r="L243" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="244" spans="1:12">
@@ -10022,7 +10022,7 @@
         <v>247670</v>
       </c>
       <c r="L244" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="245" spans="1:12">
@@ -10060,7 +10060,7 @@
         <v>158127</v>
       </c>
       <c r="L245" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="246" spans="1:12">
@@ -10098,7 +10098,7 @@
         <v>83452</v>
       </c>
       <c r="L246" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="247" spans="1:12">
@@ -10136,7 +10136,7 @@
         <v>251546</v>
       </c>
       <c r="L247" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="248" spans="1:12">
@@ -10174,7 +10174,7 @@
         <v>154483</v>
       </c>
       <c r="L248" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="249" spans="1:12">
@@ -10212,7 +10212,7 @@
         <v>83310</v>
       </c>
       <c r="L249" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="250" spans="1:12">
@@ -10250,7 +10250,7 @@
         <v>255615</v>
       </c>
       <c r="L250" s="8" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -10262,9 +10262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P250"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A250" sqref="A1:A250"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -10288,52 +10286,52 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="N1" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -16188,7 +16186,7 @@
     </row>
     <row r="119" spans="1:16">
       <c r="A119" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>3</v>
@@ -16238,7 +16236,7 @@
     </row>
     <row r="120" spans="1:16">
       <c r="A120" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>2</v>
@@ -16288,7 +16286,7 @@
     </row>
     <row r="121" spans="1:16">
       <c r="A121" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>0</v>
@@ -22795,8 +22793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E250"/>
   <sheetViews>
-    <sheetView topLeftCell="A222" workbookViewId="0">
-      <selection sqref="A1:A250"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="A225" sqref="A225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22810,19 +22808,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -24816,7 +24814,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>3</v>
@@ -24833,7 +24831,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>2</v>
@@ -24850,7 +24848,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>0</v>

</xml_diff>